<commit_message>
Wind Fetching Still Not Working, Bakcking Up
</commit_message>
<xml_diff>
--- a/player_pos_aob.xlsx
+++ b/player_pos_aob.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clib_\OneDrive\Desktop\SHAPER\PROJECTS\DDTANK_AIMBOT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0E8506-2C98-4482-A0AF-50A081C0AFC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B989AD0E-99EE-457E-9CF6-61EC7538A02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="6" xr2:uid="{E1B21AB3-602C-4857-98B6-45335151F785}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8478" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8480" uniqueCount="164">
   <si>
     <t>0C</t>
   </si>
@@ -50098,8 +50098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8D82937-C4A6-4611-8B0F-070A8489E0D3}">
   <dimension ref="A1:QV40"/>
   <sheetViews>
-    <sheetView topLeftCell="PJ2" workbookViewId="0">
-      <selection activeCell="QV2" sqref="QV2"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54912,7 +54912,7 @@
   <dimension ref="A1:QV40"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A14" sqref="A13:A14"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59733,8 +59733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8815182-3B21-4B0A-BB47-ABDD77E8A2AF}">
   <dimension ref="A1:QV40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="DL13" sqref="A13:DL13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59742,6 +59742,8 @@
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:464" x14ac:dyDescent="0.25">
@@ -69971,15 +69973,21 @@
         <v>162</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>152</v>
       </c>
       <c r="D30" t="s">
         <v>153</v>
       </c>
+      <c r="I30" t="s">
+        <v>152</v>
+      </c>
+      <c r="L30" t="s">
+        <v>153</v>
+      </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0</v>
       </c>
@@ -69992,8 +70000,17 @@
       <c r="E31">
         <v>4284984423</v>
       </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>4281430128</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -70006,8 +70023,17 @@
       <c r="E32">
         <v>4281555032</v>
       </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>4278190080</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2</v>
       </c>
@@ -70020,8 +70046,17 @@
       <c r="E33">
         <v>4294955130</v>
       </c>
+      <c r="I33">
+        <v>2</v>
+      </c>
+      <c r="J33">
+        <v>4280973432</v>
+      </c>
+      <c r="L33">
+        <v>2</v>
+      </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3</v>
       </c>
@@ -70034,8 +70069,17 @@
       <c r="E34">
         <v>4290735726</v>
       </c>
+      <c r="I34">
+        <v>3</v>
+      </c>
+      <c r="J34">
+        <v>4288102464</v>
+      </c>
+      <c r="L34">
+        <v>3</v>
+      </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4</v>
       </c>
@@ -70048,8 +70092,17 @@
       <c r="E35" t="s">
         <v>163</v>
       </c>
+      <c r="I35">
+        <v>4</v>
+      </c>
+      <c r="J35">
+        <v>4282532480</v>
+      </c>
+      <c r="L35">
+        <v>4</v>
+      </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>5</v>
       </c>
@@ -70062,8 +70115,17 @@
       <c r="E36">
         <v>4283401295</v>
       </c>
+      <c r="I36">
+        <v>5</v>
+      </c>
+      <c r="J36">
+        <v>4282941568</v>
+      </c>
+      <c r="L36">
+        <v>5</v>
+      </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>6</v>
       </c>
@@ -70076,8 +70138,17 @@
       <c r="E37">
         <v>4278718472</v>
       </c>
+      <c r="I37">
+        <v>6</v>
+      </c>
+      <c r="J37">
+        <v>4278190080</v>
+      </c>
+      <c r="L37">
+        <v>6</v>
+      </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>7</v>
       </c>
@@ -70090,8 +70161,17 @@
       <c r="E38">
         <v>4290222949</v>
       </c>
+      <c r="I38">
+        <v>7</v>
+      </c>
+      <c r="J38">
+        <v>4286611515</v>
+      </c>
+      <c r="L38">
+        <v>7</v>
+      </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>8</v>
       </c>
@@ -70104,8 +70184,17 @@
       <c r="E39">
         <v>4293388144</v>
       </c>
+      <c r="I39">
+        <v>8</v>
+      </c>
+      <c r="J39">
+        <v>4280564260</v>
+      </c>
+      <c r="L39">
+        <v>8</v>
+      </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>9</v>
       </c>
@@ -70117,6 +70206,15 @@
       </c>
       <c r="E40">
         <v>4285756335</v>
+      </c>
+      <c r="I40">
+        <v>9</v>
+      </c>
+      <c r="J40">
+        <v>4280231711</v>
+      </c>
+      <c r="L40">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>